<commit_message>
Updated the Sprint 8 Code Compare Report
</commit_message>
<xml_diff>
--- a/Documentation/Monthly Deliverables/Collaborative Development Package/Sprint 8/Sprint 8 Code Compare Report.xlsx
+++ b/Documentation/Monthly Deliverables/Collaborative Development Package/Sprint 8/Sprint 8 Code Compare Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dormand\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dormand\Documents\GitHub\Aug_22_1\Documentation\Monthly Deliverables\Collaborative Development Package\Sprint 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="64">
   <si>
     <t>Filename</t>
   </si>
@@ -135,6 +135,87 @@
   </si>
   <si>
     <t>Compare C:\Users\dormand\Documents\GitHub\July_28_2016\Code with C:\Users\dormand\Documents\GitHub\Aug_22_2016\Code</t>
+  </si>
+  <si>
+    <t>Claim.java</t>
+  </si>
+  <si>
+    <t>bcds-api\src\main\java\gov\va\vba\domain</t>
+  </si>
+  <si>
+    <t>Right only:</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>ClaimDataService.java</t>
+  </si>
+  <si>
+    <t>bcds-impl\src\main\java\gov\va\vba\service\data</t>
+  </si>
+  <si>
+    <t>bcds-persistence\src\main\java\gov\va\vba\persistence\entity</t>
+  </si>
+  <si>
+    <t>ClaimRepository.java</t>
+  </si>
+  <si>
+    <t>bcds-persistence\src\main\java\gov\va\vba\persistence\repository</t>
+  </si>
+  <si>
+    <t>ClaimResource.java</t>
+  </si>
+  <si>
+    <t>bcds-web\src\main\java\gov\va\vba\web\rest</t>
+  </si>
+  <si>
+    <t>BCDS-Image.jpg</t>
+  </si>
+  <si>
+    <t>bcds-web\src\main\webapp\assets\images</t>
+  </si>
+  <si>
+    <t>jpg</t>
+  </si>
+  <si>
+    <t>BCDS_LoginPage.jpg</t>
+  </si>
+  <si>
+    <t>BCDSS_Header.png</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>admin.controller.js</t>
+  </si>
+  <si>
+    <t>bcds-web\src\main\webapp\scripts\app\admin</t>
+  </si>
+  <si>
+    <t>claims.controller.js</t>
+  </si>
+  <si>
+    <t>bcds-web\src\main\webapp\scripts\app\claims</t>
+  </si>
+  <si>
+    <t>footer.html</t>
+  </si>
+  <si>
+    <t>rater.controller.js</t>
+  </si>
+  <si>
+    <t>modeler.controller.js</t>
+  </si>
+  <si>
+    <t>tab.controller.js</t>
+  </si>
+  <si>
+    <t>claim.service.js</t>
+  </si>
+  <si>
+    <t>bcds-web\src\main\webapp\scripts\components\entities\lookup|claim</t>
   </si>
 </sst>
 </file>
@@ -567,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="72.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,6 +1001,312 @@
         <v>15</v>
       </c>
     </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>